<commit_message>
Update Stakeholderanalyse Tabelle .xlsx
</commit_message>
<xml_diff>
--- a/Artefakte/Stakeholder/Stakeholderanalyse Tabelle .xlsx
+++ b/Artefakte/Stakeholder/Stakeholderanalyse Tabelle .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deryacoban/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B953BC8C-6A5C-2C4E-884C-EEE1C574CDDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FDB0A8-8FC2-E646-AC74-212D1DB0287F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{29C31C9A-3019-3A48-ACAA-522940A79B0F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Anspruch</t>
+  </si>
+  <si>
+    <t>Anrecht</t>
   </si>
   <si>
     <t>Bezeichnung = “Eine Einzelperson oder Unternehmen/Organisation”</t>
@@ -103,9 +106,6 @@
     <t>Als Familie muss man Wissen und Erfahrung verfügbar haben, um dies der nächsten Generation aneignen zu können</t>
   </si>
   <si>
-    <t>Als ältere Generation möchte man die spezielle Zutaten wissen, um die Rezepte weitergeben zu können</t>
-  </si>
-  <si>
     <t>an größere Schrift im System</t>
   </si>
   <si>
@@ -129,6 +129,25 @@
   </si>
   <si>
     <t>Als jüngere Generation möchte man sein Wissen über neue Rezepte mitteilen, um die ältere Generation abholen zu können</t>
+  </si>
+  <si>
+    <t>Benutzer</t>
+  </si>
+  <si>
+    <t>auf genaue Angaben vom Rezept</t>
+  </si>
+  <si>
+    <t>Als Benutzer muss man genaue Angaben verfügbar haben, um das Rezept exakt nachkochen zu können</t>
+  </si>
+  <si>
+    <t>Als ältere Generation möchte man die speziellen Zutaten kennen, um die Rezepte weitergeben zu können</t>
+  </si>
+  <si>
+    <t>einfach bedienbares System</t>
+  </si>
+  <si>
+    <t>Als ältere Generation möchte man ein einfach bedienbares System haben, um die Rezepte 
+problemlos eintragen zu können</t>
   </si>
 </sst>
 </file>
@@ -594,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24579F41-1E4D-5A4D-86F8-7A2E20781EF3}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,7 +625,7 @@
     <col min="4" max="4" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -620,7 +639,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
@@ -633,7 +652,7 @@
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:16" ht="60" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="70" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -641,13 +660,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
@@ -660,7 +679,7 @@
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -668,13 +687,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
@@ -687,7 +706,7 @@
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -695,10 +714,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -712,7 +731,7 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -720,10 +739,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -737,7 +756,7 @@
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -751,7 +770,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -764,7 +783,7 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -778,7 +797,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -791,7 +810,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -805,7 +824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -819,25 +838,41 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:16" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>

</xml_diff>